<commit_message>
working on a varibale in home
</commit_message>
<xml_diff>
--- a/relative.xlsx
+++ b/relative.xlsx
@@ -5,24 +5,37 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myagh\105_irm_baseline_assessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fmnya\105_irm_baseline_assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5F7F68-0CD1-4B27-A1EE-4AE698A0DDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2D4546-FAF0-4182-A25D-5649AF7E5957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="285" windowWidth="28800" windowHeight="15915" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="relative_support1" sheetId="1" r:id="rId1"/>
     <sheet name="relative_support2" sheetId="2" r:id="rId2"/>
     <sheet name="relative_support3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>N</t>
   </si>
@@ -57,22 +70,7 @@
     <t>very_much</t>
   </si>
   <si>
-    <t>36.79%</t>
-  </si>
-  <si>
     <t>relative_support3</t>
-  </si>
-  <si>
-    <t>20.75%</t>
-  </si>
-  <si>
-    <t>16.98%</t>
-  </si>
-  <si>
-    <t>2.83%</t>
-  </si>
-  <si>
-    <t>1.89%</t>
   </si>
   <si>
     <t>999_</t>
@@ -453,9 +451,9 @@
       <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -466,7 +464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -477,7 +475,7 @@
         <v>0.6321</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -488,9 +486,9 @@
         <v>0.35849999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -506,15 +504,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -525,9 +523,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>39</v>
@@ -536,7 +534,7 @@
         <v>0.3679</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -547,7 +545,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -558,7 +556,7 @@
         <v>0.22639999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -569,7 +567,7 @@
         <v>4.7199999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -580,7 +578,7 @@
         <v>3.7699999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -589,6 +587,18 @@
       </c>
       <c r="C7" s="2">
         <v>3.7699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <f>4/67</f>
+        <v>5.9701492537313432E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <f>4/106</f>
+        <v>3.7735849056603772E-2</v>
       </c>
     </row>
   </sheetData>
@@ -600,13 +610,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -615,68 +630,70 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B2">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="2">
+        <v>0.3679</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="2">
+        <v>0.20749999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="2">
+        <v>0.20749999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>0.16980000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>2.8299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
+      <c r="C7" s="2">
+        <v>1.89E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>